<commit_message>
ubah format date menjadi string di kolom tanggal_lahir file contoh_lansia.xlsx
</commit_message>
<xml_diff>
--- a/excel/contoh_lansia.xlsx
+++ b/excel/contoh_lansia.xlsx
@@ -700,17 +700,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1252,73 +1255,75 @@
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88888888888889" customWidth="1"/>
-    <col min="2" max="13" width="31.5555555555556" customWidth="1"/>
+    <col min="2" max="6" width="31.5555555555556" customWidth="1"/>
+    <col min="7" max="7" width="31.5555555555556" style="2" customWidth="1"/>
+    <col min="8" max="13" width="31.5555555555556" customWidth="1"/>
     <col min="14" max="14" width="35.4444444444444" customWidth="1"/>
     <col min="15" max="18" width="31.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="19" customHeight="1" spans="1:19">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add menu import excel disabilitas
</commit_message>
<xml_diff>
--- a/excel/contoh_lansia.xlsx
+++ b/excel/contoh_lansia.xlsx
@@ -70,7 +70,7 @@
     <t>keterangan_lainnya</t>
   </si>
   <si>
-    <t>tahun</t>
+    <t>tahun_anggaran</t>
   </si>
 </sst>
 </file>
@@ -700,20 +700,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -1254,8 +1251,8 @@
   <sheetPr/>
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1266,6 +1263,7 @@
     <col min="8" max="13" width="31.5555555555556" customWidth="1"/>
     <col min="14" max="14" width="35.4444444444444" customWidth="1"/>
     <col min="15" max="18" width="31.5555555555556" customWidth="1"/>
+    <col min="19" max="19" width="17.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="19" customHeight="1" spans="1:19">
@@ -1287,7 +1285,7 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -1323,7 +1321,7 @@
       <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>